<commit_message>
add formula manipulation system
</commit_message>
<xml_diff>
--- a/samplein.xlsx
+++ b/samplein.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">num</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formulae</t>
   </si>
   <si>
     <t xml:space="preserve">Johnny</t>
@@ -71,6 +74,7 @@
       <sz val="10"/>
       <name val="Nimbus Sans"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -92,6 +96,7 @@
       <color rgb="FF0000FF"/>
       <name val="Nimbus Sans"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -136,20 +141,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -170,75 +179,86 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>44966.7144560185</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="n">
         <v>2025</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="0" t="n">
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <f aca="false">SUM(D2,F2)</f>
+        <v>2026</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="3" t="n">
         <v>44967.712025463</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="n">
         <v>2023</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="0" t="n">
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">SUM(D3,F3)</f>
+        <v>2025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix auto user add
</commit_message>
<xml_diff>
--- a/samplein.xlsx
+++ b/samplein.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -37,12 +37,6 @@
     <t xml:space="preserve">WPI email</t>
   </si>
   <si>
-    <t xml:space="preserve">num</t>
-  </si>
-  <si>
-    <t xml:space="preserve">formulae</t>
-  </si>
-  <si>
     <t xml:space="preserve">Johnny</t>
   </si>
   <si>
@@ -59,6 +53,15 @@
   </si>
   <si>
     <t xml:space="preserve">jhendrix@wpi.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lady</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">queen@wpi.edu</t>
   </si>
 </sst>
 </file>
@@ -179,16 +182,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -207,65 +210,69 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
         <v>44966.7144560185</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>2025</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <f aca="false">SUM(D2,F2)</f>
-        <v>2026</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
         <v>44967.712025463</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>2023</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <v>44967.7536921296</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <f aca="false">SUM(D3,F3)</f>
-        <v>2025</v>
+      <c r="D4" s="0" t="n">
+        <v>2024</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="jappleseed@wpi.edu"/>
     <hyperlink ref="E3" r:id="rId2" display="jhendrix@wpi.edu"/>
+    <hyperlink ref="E4" r:id="rId3" display="queen@wpi.edu"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>